<commit_message>
se realizo correctamente la migracion a la nueva interfaz
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -29,12 +29,22 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004CE308"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +65,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +493,12 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Vencimiento</t>
+          <t>Vencimiento_Formateada</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
         </is>
       </c>
     </row>
@@ -519,7 +536,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="2" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
@@ -532,6 +549,11 @@
       <c r="J2" t="inlineStr">
         <is>
           <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>
@@ -569,7 +591,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -582,6 +604,11 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>17/01/2023</t>
+        </is>
+      </c>
+      <c r="K3" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>
@@ -619,7 +646,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -632,6 +659,11 @@
       <c r="J4" t="inlineStr">
         <is>
           <t>20/01/2023</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>
@@ -669,7 +701,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -682,6 +714,11 @@
       <c r="J5" t="inlineStr">
         <is>
           <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K5" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>
@@ -719,7 +756,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>5000</t>
         </is>
@@ -732,6 +769,11 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>
@@ -746,7 +788,7 @@
           <t xml:space="preserve">francisco </t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="2" t="n">
         <v>123</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -769,7 +811,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -782,6 +824,11 @@
       <c r="J7" t="inlineStr">
         <is>
           <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>
@@ -819,7 +866,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -832,6 +879,11 @@
       <c r="J8" t="inlineStr">
         <is>
           <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego la opcion de busqueda con resultado filtrado
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -866,9 +866,9 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H8" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">

</xml_diff>

<commit_message>
se agrego el interfaz de acceso de clientes
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -538,22 +538,22 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>4500</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>22/01/2024</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>20/01/2024</t>
-        </is>
-      </c>
-      <c r="K2" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>22/02/2024</t>
+        </is>
+      </c>
+      <c r="K2" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>
@@ -884,6 +884,61 @@
       <c r="K8" s="2" t="inlineStr">
         <is>
           <t>Vencido</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>fre</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>julieta</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>12345671</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>213524896</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>gasdgsad</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>13/10/05</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>pase libre</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>-1000</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>22/01/2024</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>22/02/2024</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego el menu de ficha de socio
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -70,8 +70,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -538,7 +538,7 @@
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
-          <t>4500</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -548,10 +548,10 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>22/02/2024</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="inlineStr">
+          <t>25/01/2024</t>
+        </is>
+      </c>
+      <c r="K2" s="2" t="inlineStr">
         <is>
           <t>Regular</t>
         </is>
@@ -591,7 +591,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="H3" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -606,7 +606,7 @@
           <t>17/01/2023</t>
         </is>
       </c>
-      <c r="K3" s="2" t="inlineStr">
+      <c r="K3" s="3" t="inlineStr">
         <is>
           <t>Vencido</t>
         </is>
@@ -646,7 +646,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="H4" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -661,7 +661,7 @@
           <t>20/01/2023</t>
         </is>
       </c>
-      <c r="K4" s="2" t="inlineStr">
+      <c r="K4" s="3" t="inlineStr">
         <is>
           <t>Vencido</t>
         </is>
@@ -701,7 +701,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H5" s="3" t="inlineStr">
+      <c r="H5" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -716,7 +716,7 @@
           <t>20/01/2024</t>
         </is>
       </c>
-      <c r="K5" s="2" t="inlineStr">
+      <c r="K5" s="3" t="inlineStr">
         <is>
           <t>Vencido</t>
         </is>
@@ -756,7 +756,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H6" s="2" t="inlineStr">
+      <c r="H6" s="3" t="inlineStr">
         <is>
           <t>5000</t>
         </is>
@@ -771,7 +771,7 @@
           <t>20/01/2024</t>
         </is>
       </c>
-      <c r="K6" s="2" t="inlineStr">
+      <c r="K6" s="3" t="inlineStr">
         <is>
           <t>Vencido</t>
         </is>
@@ -788,7 +788,7 @@
           <t xml:space="preserve">francisco </t>
         </is>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>123</v>
       </c>
       <c r="D7" t="inlineStr">
@@ -811,7 +811,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr">
+      <c r="H7" s="2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -826,7 +826,7 @@
           <t>20/01/2024</t>
         </is>
       </c>
-      <c r="K7" s="2" t="inlineStr">
+      <c r="K7" s="3" t="inlineStr">
         <is>
           <t>Vencido</t>
         </is>
@@ -866,7 +866,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H8" s="2" t="inlineStr">
+      <c r="H8" s="3" t="inlineStr">
         <is>
           <t>100</t>
         </is>
@@ -881,7 +881,7 @@
           <t>20/01/2024</t>
         </is>
       </c>
-      <c r="K8" s="2" t="inlineStr">
+      <c r="K8" s="3" t="inlineStr">
         <is>
           <t>Vencido</t>
         </is>
@@ -921,7 +921,7 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H9" s="3" t="inlineStr">
+      <c r="H9" s="2" t="inlineStr">
         <is>
           <t>-1000</t>
         </is>
@@ -936,7 +936,7 @@
           <t>22/02/2024</t>
         </is>
       </c>
-      <c r="K9" s="3" t="inlineStr">
+      <c r="K9" s="2" t="inlineStr">
         <is>
           <t>Regular</t>
         </is>

</xml_diff>

<commit_message>
se agrego el menu de caja
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -528,7 +528,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>10/26/02</t>
+          <t>10/10/2002</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -578,12 +578,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>martingaido00@gmail.com</t>
+          <t>martingaido0@gmail.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>19/11/03</t>
+          <t>18/11/2003</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -638,7 +638,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11/10/02</t>
+          <t>11/10/2002</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -693,7 +693,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2/10/03</t>
+          <t>2/10/2003</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -701,9 +701,9 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H5" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>5/10/89</t>
+          <t>5/10/1989</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>24/10/03</t>
+          <t>24/10/2003</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -858,7 +858,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>9/5/77</t>
+          <t>9/5/1977</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">

</xml_diff>

<commit_message>
se agrego la opcion de seleccionar el vencimiento si va a ser actual o usando el vencimiento anterior
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -591,24 +591,24 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>17/12/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>17/01/2023</t>
-        </is>
-      </c>
-      <c r="K3" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>06/03/2024</t>
+        </is>
+      </c>
+      <c r="K3" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>
@@ -646,24 +646,24 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H4" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>1000</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>20/01/2023</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>06/03/2024</t>
+        </is>
+      </c>
+      <c r="K4" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>
@@ -866,24 +866,24 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>100</t>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>-900</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>20/01/2024</t>
-        </is>
-      </c>
-      <c r="K8" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>20/02/2024</t>
+        </is>
+      </c>
+      <c r="K8" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego la opcion de dar de baja un cliente
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,30 +560,30 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>gaido</t>
+          <t>rodriguez</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>martin</t>
+          <t>julio</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>45087672</v>
+        <v>98765431</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3533499701</t>
+          <t>2561485</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>martingaido0@gmail.com</t>
+          <t>asdgsda</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>18/11/2003</t>
+          <t>06/10/2004</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -591,19 +591,19 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="H3" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>08/02/2024</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>06/03/2024</t>
+          <t>08/03/2024</t>
         </is>
       </c>
       <c r="K3" s="3" t="inlineStr">
@@ -615,30 +615,30 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>gonzales</t>
+          <t>gaido</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>matiass</t>
+          <t>marcos</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>12345678</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>3533353342</t>
+        <v>98765432</v>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>35364</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>fasd@gmaila.com</t>
+          <t>fsag</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>11/10/2002</t>
+          <t>16/10/2008</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -648,17 +648,17 @@
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>06/02/2024</t>
+          <t>08/02/2024</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>06/03/2024</t>
+          <t>08/03/2024</t>
         </is>
       </c>
       <c r="K4" s="3" t="inlineStr">
@@ -670,30 +670,30 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cabred</t>
+          <t>gaido</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>kevin</t>
+          <t>martin</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>87654321</v>
+        <v>45087672</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3533123456</t>
+          <t>3533499701</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>kevin@gmail.com</t>
+          <t>martingaido0@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2/10/2003</t>
+          <t>18/11/2003</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -703,52 +703,52 @@
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>100</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>20/01/2024</t>
-        </is>
-      </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>06/03/2024</t>
+        </is>
+      </c>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>gaido</t>
+          <t>gonzales</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>cristian</t>
+          <t>matiass</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>45875236</v>
+        <v>12345678</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3533499706</t>
+          <t>3533353342</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>cristian@gmail.com</t>
+          <t>fasd@gmaila.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>5/10/1989</t>
+          <t>11/10/2002</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -758,52 +758,52 @@
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>500</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>06/02/2024</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>20/01/2024</t>
-        </is>
-      </c>
-      <c r="K6" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>06/03/2024</t>
+        </is>
+      </c>
+      <c r="K6" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>sierra</t>
+          <t>cabred</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t xml:space="preserve">francisco </t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>123</v>
+          <t>kevin</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>87654321</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3533123458</t>
+          <t>3533123456</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>fran@gmail.com</t>
+          <t>kevin@gmail.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>24/10/2003</t>
+          <t>2/10/2003</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -811,9 +811,9 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H7" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -835,53 +835,163 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>gaido</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>cristian</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>45875236</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>3533499706</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>cristian@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5/10/1989</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>pase libre</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>20/12/2023</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sierra</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">francisco </t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>12365498</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>3533123458</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>fran@gmail.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>24/10/2003</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>pase libre</t>
+        </is>
+      </c>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>20/12/2023</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>20/01/2024</t>
+        </is>
+      </c>
+      <c r="K9" s="2" t="inlineStr">
+        <is>
+          <t>Vencido</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Rodriguez</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>Carina</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C10" t="n">
         <v>25810173</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>3533417461</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>carinadelvaller@gmail.com</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>9/5/1977</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H8" s="3" t="inlineStr">
-        <is>
-          <t>-900</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="H10" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>06/02/2024</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>20/02/2024</t>
         </is>
       </c>
-      <c r="K8" s="3" t="inlineStr">
+      <c r="K10" s="3" t="inlineStr">
         <is>
           <t>Regular</t>
         </is>

</xml_diff>

<commit_message>
se re acomodaron todos los archivos en componentes
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -518,7 +518,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3533698547</t>
+          <t>3537651910</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -548,7 +548,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>22/02/2024</t>
+          <t>15/02/2024</t>
         </is>
       </c>
       <c r="K2" s="3" t="inlineStr">
@@ -591,9 +591,9 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H3" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>06/03/2024</t>
+          <t>13/02/2024</t>
         </is>
       </c>
       <c r="K5" s="3" t="inlineStr">
@@ -921,24 +921,24 @@
           <t>pase libre</t>
         </is>
       </c>
-      <c r="H9" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>6500</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>20/12/2023</t>
+          <t>11/02/2024</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>20/01/2024</t>
-        </is>
-      </c>
-      <c r="K9" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+          <t>11/03/2024</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "hecho por martin"
</commit_message>
<xml_diff>
--- a/datos_clientes.xlsx
+++ b/datos_clientes.xlsx
@@ -716,9 +716,9 @@
           <t>13/02/2024</t>
         </is>
       </c>
-      <c r="K5" s="2" t="inlineStr">
-        <is>
-          <t>Vencido</t>
+      <c r="K5" s="3" t="inlineStr">
+        <is>
+          <t>Regular</t>
         </is>
       </c>
     </row>

</xml_diff>